<commit_message>
Added pandas and arguments
Started data handling using pandas to import xlsx file data. started writing high level functions to read/parse xlsx data.

modified excel files to standardize column names
</commit_message>
<xml_diff>
--- a/individual_treasure_tables.xlsx
+++ b/individual_treasure_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D6B16-CBE1-41B2-AA4A-957455B6E5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A4E96-3B8F-492A-AC31-67527155D694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9790" yWindow="2560" windowWidth="20820" windowHeight="17410" activeTab="3" xr2:uid="{095ACC5E-2FB4-4AB2-A703-98B948D267C9}"/>
+    <workbookView xWindow="1830" yWindow="1180" windowWidth="20820" windowHeight="17410" activeTab="3" xr2:uid="{095ACC5E-2FB4-4AB2-A703-98B948D267C9}"/>
   </bookViews>
   <sheets>
     <sheet name="CR 0-4" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="48">
   <si>
     <t>copper</t>
   </si>
@@ -75,9 +75,6 @@
     <t>2d6x10</t>
   </si>
   <si>
-    <t>1d6 x 100</t>
-  </si>
-  <si>
     <t>1d6x100</t>
   </si>
   <si>
@@ -183,7 +180,7 @@
     <t>1d6x1000</t>
   </si>
   <si>
-    <t>2d6 x 100</t>
+    <t>Roll</t>
   </si>
 </sst>
 </file>
@@ -552,13 +549,16 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P92" sqref="P92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1399,6 +1399,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1993,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
@@ -2001,7 +2004,7 @@
         <v>62</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>11</v>
@@ -2012,7 +2015,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>11</v>
@@ -2023,7 +2026,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>11</v>
@@ -2034,7 +2037,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>11</v>
@@ -2045,7 +2048,7 @@
         <v>66</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>11</v>
@@ -2056,7 +2059,7 @@
         <v>67</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>11</v>
@@ -2067,7 +2070,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>11</v>
@@ -2078,7 +2081,7 @@
         <v>69</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>11</v>
@@ -2089,7 +2092,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>11</v>
@@ -2100,7 +2103,7 @@
         <v>71</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -2108,7 +2111,7 @@
         <v>72</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -2116,7 +2119,7 @@
         <v>73</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2124,7 +2127,7 @@
         <v>74</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -2132,7 +2135,7 @@
         <v>75</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -2140,7 +2143,7 @@
         <v>76</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -2148,7 +2151,7 @@
         <v>77</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -2156,7 +2159,7 @@
         <v>78</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -2164,7 +2167,7 @@
         <v>79</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -2172,7 +2175,7 @@
         <v>80</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2180,7 +2183,7 @@
         <v>81</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2188,7 +2191,7 @@
         <v>82</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2196,7 +2199,7 @@
         <v>83</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -2204,7 +2207,7 @@
         <v>84</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -2212,7 +2215,7 @@
         <v>85</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -2220,7 +2223,7 @@
         <v>86</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -2228,7 +2231,7 @@
         <v>87</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2236,7 +2239,7 @@
         <v>88</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2244,7 +2247,7 @@
         <v>89</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2252,7 +2255,7 @@
         <v>90</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -2260,7 +2263,7 @@
         <v>91</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -2268,7 +2271,7 @@
         <v>92</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -2276,7 +2279,7 @@
         <v>93</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2284,7 +2287,7 @@
         <v>94</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2292,7 +2295,7 @@
         <v>95</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -2362,13 +2365,16 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K96" sqref="K96"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2404,7 +2410,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -2415,7 +2421,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -2426,7 +2432,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2437,7 +2443,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -2448,7 +2454,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -2459,7 +2465,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -2470,7 +2476,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2481,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2492,7 +2498,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2503,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2514,7 +2520,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -2525,7 +2531,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2536,7 +2542,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2547,7 +2553,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2558,7 +2564,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2569,7 +2575,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2580,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2591,7 +2597,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2602,7 +2608,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2610,10 +2616,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -2621,10 +2627,10 @@
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -2632,10 +2638,10 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -2643,10 +2649,10 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2654,10 +2660,10 @@
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -2665,10 +2671,10 @@
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -2676,10 +2682,10 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -2687,10 +2693,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -2698,10 +2704,10 @@
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -2709,10 +2715,10 @@
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -2720,10 +2726,10 @@
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -2731,10 +2737,10 @@
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -2742,10 +2748,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -2753,10 +2759,10 @@
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -2764,10 +2770,10 @@
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -2775,10 +2781,10 @@
         <v>36</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
         <v>15</v>
-      </c>
-      <c r="F37" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -2786,10 +2792,10 @@
         <v>37</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" t="s">
         <v>15</v>
-      </c>
-      <c r="F38" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2797,10 +2803,10 @@
         <v>38</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" t="s">
         <v>15</v>
-      </c>
-      <c r="F39" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2808,10 +2814,10 @@
         <v>39</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" t="s">
         <v>15</v>
-      </c>
-      <c r="F40" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2819,10 +2825,10 @@
         <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
         <v>15</v>
-      </c>
-      <c r="F41" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -2830,10 +2836,10 @@
         <v>41</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" t="s">
         <v>15</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -2841,10 +2847,10 @@
         <v>42</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" t="s">
         <v>15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -2852,10 +2858,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" t="s">
         <v>15</v>
-      </c>
-      <c r="F44" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -2863,10 +2869,10 @@
         <v>44</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
         <v>15</v>
-      </c>
-      <c r="F45" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -2874,10 +2880,10 @@
         <v>45</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
         <v>15</v>
-      </c>
-      <c r="F46" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -2885,10 +2891,10 @@
         <v>46</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
         <v>15</v>
-      </c>
-      <c r="F47" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -2896,10 +2902,10 @@
         <v>47</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
         <v>15</v>
-      </c>
-      <c r="F48" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2907,10 +2913,10 @@
         <v>48</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" t="s">
         <v>15</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2918,10 +2924,10 @@
         <v>49</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
         <v>15</v>
-      </c>
-      <c r="F50" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2929,10 +2935,10 @@
         <v>50</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
         <v>15</v>
-      </c>
-      <c r="F51" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2940,10 +2946,10 @@
         <v>51</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="s">
         <v>15</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2951,10 +2957,10 @@
         <v>52</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
         <v>15</v>
-      </c>
-      <c r="F53" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2962,10 +2968,10 @@
         <v>53</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" t="s">
         <v>15</v>
-      </c>
-      <c r="F54" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2973,10 +2979,10 @@
         <v>54</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
         <v>15</v>
-      </c>
-      <c r="F55" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2984,10 +2990,10 @@
         <v>55</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" t="s">
         <v>15</v>
-      </c>
-      <c r="F56" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2995,10 +3001,10 @@
         <v>56</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" t="s">
         <v>15</v>
-      </c>
-      <c r="F57" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -3006,10 +3012,10 @@
         <v>57</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" t="s">
         <v>15</v>
-      </c>
-      <c r="F58" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -3017,10 +3023,10 @@
         <v>58</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
         <v>15</v>
-      </c>
-      <c r="F59" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -3028,10 +3034,10 @@
         <v>59</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" t="s">
         <v>15</v>
-      </c>
-      <c r="F60" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -3039,10 +3045,10 @@
         <v>60</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" t="s">
         <v>15</v>
-      </c>
-      <c r="F61" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -3050,10 +3056,10 @@
         <v>61</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" t="s">
         <v>15</v>
-      </c>
-      <c r="F62" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -3061,10 +3067,10 @@
         <v>62</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" t="s">
         <v>15</v>
-      </c>
-      <c r="F63" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -3072,10 +3078,10 @@
         <v>63</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" t="s">
         <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -3083,10 +3089,10 @@
         <v>64</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" t="s">
         <v>15</v>
-      </c>
-      <c r="F65" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -3094,10 +3100,10 @@
         <v>65</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" t="s">
         <v>15</v>
-      </c>
-      <c r="F66" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -3105,10 +3111,10 @@
         <v>66</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" t="s">
         <v>15</v>
-      </c>
-      <c r="F67" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -3116,10 +3122,10 @@
         <v>67</v>
       </c>
       <c r="E68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" t="s">
         <v>15</v>
-      </c>
-      <c r="F68" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -3127,10 +3133,10 @@
         <v>68</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" t="s">
         <v>15</v>
-      </c>
-      <c r="F69" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -3138,10 +3144,10 @@
         <v>69</v>
       </c>
       <c r="E70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" t="s">
         <v>15</v>
-      </c>
-      <c r="F70" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -3149,10 +3155,10 @@
         <v>70</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" t="s">
         <v>15</v>
-      </c>
-      <c r="F71" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -3160,10 +3166,10 @@
         <v>71</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" t="s">
         <v>15</v>
-      </c>
-      <c r="F72" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -3171,10 +3177,10 @@
         <v>72</v>
       </c>
       <c r="E73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" t="s">
         <v>15</v>
-      </c>
-      <c r="F73" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -3182,10 +3188,10 @@
         <v>73</v>
       </c>
       <c r="E74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" t="s">
         <v>15</v>
-      </c>
-      <c r="F74" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -3193,10 +3199,10 @@
         <v>74</v>
       </c>
       <c r="E75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
         <v>15</v>
-      </c>
-      <c r="F75" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -3204,10 +3210,10 @@
         <v>75</v>
       </c>
       <c r="E76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" t="s">
         <v>15</v>
-      </c>
-      <c r="F76" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -3215,7 +3221,7 @@
         <v>76</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
@@ -3226,7 +3232,7 @@
         <v>77</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
@@ -3237,7 +3243,7 @@
         <v>78</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F79" t="s">
         <v>11</v>
@@ -3248,7 +3254,7 @@
         <v>79</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F80" t="s">
         <v>11</v>
@@ -3259,7 +3265,7 @@
         <v>80</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F81" t="s">
         <v>11</v>
@@ -3270,7 +3276,7 @@
         <v>81</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F82" t="s">
         <v>11</v>
@@ -3281,7 +3287,7 @@
         <v>82</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F83" t="s">
         <v>11</v>
@@ -3292,7 +3298,7 @@
         <v>83</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F84" t="s">
         <v>11</v>
@@ -3303,7 +3309,7 @@
         <v>84</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F85" t="s">
         <v>11</v>
@@ -3314,7 +3320,7 @@
         <v>85</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -3325,7 +3331,7 @@
         <v>86</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F87" t="s">
         <v>11</v>
@@ -3336,7 +3342,7 @@
         <v>87</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
@@ -3347,7 +3353,7 @@
         <v>88</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F89" t="s">
         <v>11</v>
@@ -3358,7 +3364,7 @@
         <v>89</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -3369,7 +3375,7 @@
         <v>90</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F91" t="s">
         <v>11</v>
@@ -3380,7 +3386,7 @@
         <v>91</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
@@ -3391,7 +3397,7 @@
         <v>92</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F93" t="s">
         <v>11</v>
@@ -3402,7 +3408,7 @@
         <v>93</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F94" t="s">
         <v>11</v>
@@ -3413,7 +3419,7 @@
         <v>94</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F95" t="s">
         <v>11</v>
@@ -3424,7 +3430,7 @@
         <v>95</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F96" t="s">
         <v>11</v>
@@ -3435,7 +3441,7 @@
         <v>96</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F97" t="s">
         <v>11</v>
@@ -3446,7 +3452,7 @@
         <v>97</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F98" t="s">
         <v>11</v>
@@ -3457,7 +3463,7 @@
         <v>98</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s">
         <v>11</v>
@@ -3468,7 +3474,7 @@
         <v>99</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
@@ -3479,7 +3485,7 @@
         <v>100</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F101" t="s">
         <v>11</v>
@@ -3496,13 +3502,16 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I94" sqref="I94"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3524,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3535,10 +3544,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3546,10 +3555,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3557,10 +3566,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3568,10 +3577,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3579,10 +3588,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3590,10 +3599,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3601,10 +3610,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3612,10 +3621,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3623,10 +3632,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3634,10 +3643,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3645,10 +3654,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
         <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3656,10 +3665,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
         <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3667,10 +3676,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
         <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3678,10 +3687,10 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
         <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -3689,7 +3698,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -3700,7 +3709,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -3711,7 +3720,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -3722,7 +3731,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -3733,7 +3742,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -3744,7 +3753,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -3755,7 +3764,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -3766,7 +3775,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -3777,7 +3786,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -3788,7 +3797,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
@@ -3799,7 +3808,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -3810,7 +3819,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -3821,7 +3830,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -3832,7 +3841,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -3843,7 +3852,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -3854,7 +3863,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -3865,7 +3874,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -3876,7 +3885,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -3887,7 +3896,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -3898,7 +3907,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -3909,7 +3918,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -3920,7 +3929,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -3931,7 +3940,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -3942,7 +3951,7 @@
         <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -3953,7 +3962,7 @@
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -3964,7 +3973,7 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
@@ -3975,7 +3984,7 @@
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -3986,7 +3995,7 @@
         <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -3997,7 +4006,7 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" t="s">
         <v>12</v>
@@ -4008,7 +4017,7 @@
         <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -4019,7 +4028,7 @@
         <v>46</v>
       </c>
       <c r="E47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F47" t="s">
         <v>12</v>
@@ -4030,7 +4039,7 @@
         <v>47</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -4041,7 +4050,7 @@
         <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
@@ -4052,7 +4061,7 @@
         <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -4063,7 +4072,7 @@
         <v>50</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
@@ -4074,7 +4083,7 @@
         <v>51</v>
       </c>
       <c r="E52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
@@ -4085,7 +4094,7 @@
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F53" t="s">
         <v>12</v>
@@ -4096,7 +4105,7 @@
         <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -4107,7 +4116,7 @@
         <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -4118,7 +4127,7 @@
         <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
@@ -4129,10 +4138,10 @@
         <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -4140,10 +4149,10 @@
         <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -4151,10 +4160,10 @@
         <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F59" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -4162,10 +4171,10 @@
         <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F60" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -4173,10 +4182,10 @@
         <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F61" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -4184,10 +4193,10 @@
         <v>61</v>
       </c>
       <c r="E62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F62" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -4195,10 +4204,10 @@
         <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F63" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -4206,10 +4215,10 @@
         <v>63</v>
       </c>
       <c r="E64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F64" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -4217,10 +4226,10 @@
         <v>64</v>
       </c>
       <c r="E65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F65" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -4228,10 +4237,10 @@
         <v>65</v>
       </c>
       <c r="E66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F66" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -4239,10 +4248,10 @@
         <v>66</v>
       </c>
       <c r="E67" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F67" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -4250,10 +4259,10 @@
         <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F68" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -4261,10 +4270,10 @@
         <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F69" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -4272,10 +4281,10 @@
         <v>69</v>
       </c>
       <c r="E70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F70" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -4283,10 +4292,10 @@
         <v>70</v>
       </c>
       <c r="E71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F71" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -4294,10 +4303,10 @@
         <v>71</v>
       </c>
       <c r="E72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F72" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -4305,10 +4314,10 @@
         <v>72</v>
       </c>
       <c r="E73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F73" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -4316,10 +4325,10 @@
         <v>73</v>
       </c>
       <c r="E74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F74" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -4327,10 +4336,10 @@
         <v>74</v>
       </c>
       <c r="E75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F75" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -4338,10 +4347,10 @@
         <v>75</v>
       </c>
       <c r="E76" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F76" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -4349,10 +4358,10 @@
         <v>76</v>
       </c>
       <c r="E77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F77" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -4360,10 +4369,10 @@
         <v>77</v>
       </c>
       <c r="E78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -4371,10 +4380,10 @@
         <v>78</v>
       </c>
       <c r="E79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F79" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -4382,10 +4391,10 @@
         <v>79</v>
       </c>
       <c r="E80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F80" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -4393,10 +4402,10 @@
         <v>80</v>
       </c>
       <c r="E81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F81" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -4404,10 +4413,10 @@
         <v>81</v>
       </c>
       <c r="E82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F82" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -4415,10 +4424,10 @@
         <v>82</v>
       </c>
       <c r="E83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F83" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -4426,10 +4435,10 @@
         <v>83</v>
       </c>
       <c r="E84" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F84" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -4437,10 +4446,10 @@
         <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F85" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -4448,10 +4457,10 @@
         <v>85</v>
       </c>
       <c r="E86" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F86" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -4459,10 +4468,10 @@
         <v>86</v>
       </c>
       <c r="E87" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F87" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -4470,10 +4479,10 @@
         <v>87</v>
       </c>
       <c r="E88" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F88" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -4481,10 +4490,10 @@
         <v>88</v>
       </c>
       <c r="E89" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F89" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -4492,10 +4501,10 @@
         <v>89</v>
       </c>
       <c r="E90" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F90" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -4503,10 +4512,10 @@
         <v>90</v>
       </c>
       <c r="E91" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F91" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -4514,10 +4523,10 @@
         <v>91</v>
       </c>
       <c r="E92" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F92" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -4525,10 +4534,10 @@
         <v>92</v>
       </c>
       <c r="E93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F93" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -4536,10 +4545,10 @@
         <v>93</v>
       </c>
       <c r="E94" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F94" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -4547,10 +4556,10 @@
         <v>94</v>
       </c>
       <c r="E95" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F95" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -4558,10 +4567,10 @@
         <v>95</v>
       </c>
       <c r="E96" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F96" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -4569,10 +4578,10 @@
         <v>96</v>
       </c>
       <c r="E97" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F97" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -4580,10 +4589,10 @@
         <v>97</v>
       </c>
       <c r="E98" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F98" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -4591,10 +4600,10 @@
         <v>98</v>
       </c>
       <c r="E99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F99" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -4602,10 +4611,10 @@
         <v>99</v>
       </c>
       <c r="E100" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F100" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -4613,10 +4622,10 @@
         <v>100</v>
       </c>
       <c r="E101" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F101" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoard Tables and Excel Standardization
Kept working on hoard generator and modified excel tables for consistency
</commit_message>
<xml_diff>
--- a/individual_treasure_tables.xlsx
+++ b/individual_treasure_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A4E96-3B8F-492A-AC31-67527155D694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A27C4CD-B16D-4869-8FC1-78E22AE8F102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1180" windowWidth="20820" windowHeight="17410" activeTab="3" xr2:uid="{095ACC5E-2FB4-4AB2-A703-98B948D267C9}"/>
+    <workbookView xWindow="11840" yWindow="680" windowWidth="20820" windowHeight="17410" xr2:uid="{095ACC5E-2FB4-4AB2-A703-98B948D267C9}"/>
   </bookViews>
   <sheets>
     <sheet name="CR 0-4" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="20">
   <si>
     <t>copper</t>
   </si>
@@ -91,90 +91,6 @@
   </si>
   <si>
     <t>8d6x100</t>
-  </si>
-  <si>
-    <t>2d6x1001</t>
-  </si>
-  <si>
-    <t>8d6x101</t>
-  </si>
-  <si>
-    <t>2d6x1002</t>
-  </si>
-  <si>
-    <t>8d6x102</t>
-  </si>
-  <si>
-    <t>2d6x1003</t>
-  </si>
-  <si>
-    <t>8d6x103</t>
-  </si>
-  <si>
-    <t>2d6x1004</t>
-  </si>
-  <si>
-    <t>8d6x104</t>
-  </si>
-  <si>
-    <t>2d6x1005</t>
-  </si>
-  <si>
-    <t>8d6x105</t>
-  </si>
-  <si>
-    <t>2d6x1006</t>
-  </si>
-  <si>
-    <t>8d6x106</t>
-  </si>
-  <si>
-    <t>2d6x1007</t>
-  </si>
-  <si>
-    <t>8d6x107</t>
-  </si>
-  <si>
-    <t>2d6x1008</t>
-  </si>
-  <si>
-    <t>8d6x108</t>
-  </si>
-  <si>
-    <t>2d6x1009</t>
-  </si>
-  <si>
-    <t>8d6x109</t>
-  </si>
-  <si>
-    <t>2d6x1010</t>
-  </si>
-  <si>
-    <t>8d6x110</t>
-  </si>
-  <si>
-    <t>2d6x1011</t>
-  </si>
-  <si>
-    <t>8d6x111</t>
-  </si>
-  <si>
-    <t>2d6x1012</t>
-  </si>
-  <si>
-    <t>8d6x112</t>
-  </si>
-  <si>
-    <t>2d6x1013</t>
-  </si>
-  <si>
-    <t>8d6x113</t>
-  </si>
-  <si>
-    <t>2d6x1014</t>
-  </si>
-  <si>
-    <t>8d6x114</t>
   </si>
   <si>
     <t>1d6x1000</t>
@@ -548,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272E85A3-7599-4901-BC87-995CB1C3B3B6}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P92" sqref="P92"/>
     </sheetView>
   </sheetViews>
@@ -557,7 +473,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1400,7 +1316,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2373,7 +2289,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3501,16 +3417,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773EE5AC-0C3E-4256-A811-73F676C17D48}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3544,10 +3460,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3555,10 +3471,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3566,10 +3482,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3577,10 +3493,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3588,10 +3504,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3599,10 +3515,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3610,10 +3526,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3621,10 +3537,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3632,10 +3548,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3643,10 +3559,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3654,10 +3570,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3665,10 +3581,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3676,10 +3592,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3687,10 +3603,10 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -3698,7 +3614,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -3709,7 +3625,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -3720,7 +3636,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -3731,7 +3647,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -3742,7 +3658,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -3753,7 +3669,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -3764,7 +3680,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -3775,7 +3691,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -3786,7 +3702,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -3797,7 +3713,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
@@ -3808,7 +3724,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -3819,7 +3735,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -3830,7 +3746,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -3841,7 +3757,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -3852,7 +3768,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -3863,7 +3779,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -3874,7 +3790,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -3885,7 +3801,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -3896,7 +3812,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -3907,7 +3823,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -3918,7 +3834,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -3929,7 +3845,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -3940,7 +3856,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -3951,7 +3867,7 @@
         <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -3962,7 +3878,7 @@
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -3973,7 +3889,7 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
@@ -3984,7 +3900,7 @@
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -3995,7 +3911,7 @@
         <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -4006,7 +3922,7 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F45" t="s">
         <v>12</v>
@@ -4017,7 +3933,7 @@
         <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -4028,7 +3944,7 @@
         <v>46</v>
       </c>
       <c r="E47" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F47" t="s">
         <v>12</v>
@@ -4039,7 +3955,7 @@
         <v>47</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -4050,7 +3966,7 @@
         <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
@@ -4061,7 +3977,7 @@
         <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -4072,7 +3988,7 @@
         <v>50</v>
       </c>
       <c r="E51" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
@@ -4083,7 +3999,7 @@
         <v>51</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
@@ -4094,7 +4010,7 @@
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F53" t="s">
         <v>12</v>
@@ -4105,7 +4021,7 @@
         <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -4116,7 +4032,7 @@
         <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -4127,7 +4043,7 @@
         <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
@@ -4138,7 +4054,7 @@
         <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
@@ -4149,7 +4065,7 @@
         <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F58" t="s">
         <v>14</v>
@@ -4160,7 +4076,7 @@
         <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F59" t="s">
         <v>14</v>
@@ -4171,7 +4087,7 @@
         <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F60" t="s">
         <v>14</v>
@@ -4182,7 +4098,7 @@
         <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F61" t="s">
         <v>14</v>
@@ -4193,7 +4109,7 @@
         <v>61</v>
       </c>
       <c r="E62" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F62" t="s">
         <v>14</v>
@@ -4204,7 +4120,7 @@
         <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F63" t="s">
         <v>14</v>
@@ -4215,7 +4131,7 @@
         <v>63</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F64" t="s">
         <v>14</v>
@@ -4226,7 +4142,7 @@
         <v>64</v>
       </c>
       <c r="E65" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -4237,7 +4153,7 @@
         <v>65</v>
       </c>
       <c r="E66" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -4248,7 +4164,7 @@
         <v>66</v>
       </c>
       <c r="E67" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
@@ -4259,7 +4175,7 @@
         <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
@@ -4270,7 +4186,7 @@
         <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F69" t="s">
         <v>14</v>
@@ -4281,7 +4197,7 @@
         <v>69</v>
       </c>
       <c r="E70" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F70" t="s">
         <v>14</v>
@@ -4292,7 +4208,7 @@
         <v>70</v>
       </c>
       <c r="E71" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F71" t="s">
         <v>14</v>
@@ -4303,7 +4219,7 @@
         <v>71</v>
       </c>
       <c r="E72" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F72" t="s">
         <v>14</v>
@@ -4314,7 +4230,7 @@
         <v>72</v>
       </c>
       <c r="E73" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -4325,7 +4241,7 @@
         <v>73</v>
       </c>
       <c r="E74" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F74" t="s">
         <v>14</v>
@@ -4336,7 +4252,7 @@
         <v>74</v>
       </c>
       <c r="E75" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F75" t="s">
         <v>14</v>
@@ -4347,7 +4263,7 @@
         <v>75</v>
       </c>
       <c r="E76" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -4358,7 +4274,7 @@
         <v>76</v>
       </c>
       <c r="E77" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F77" t="s">
         <v>14</v>
@@ -4369,7 +4285,7 @@
         <v>77</v>
       </c>
       <c r="E78" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -4380,7 +4296,7 @@
         <v>78</v>
       </c>
       <c r="E79" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F79" t="s">
         <v>14</v>
@@ -4391,7 +4307,7 @@
         <v>79</v>
       </c>
       <c r="E80" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F80" t="s">
         <v>14</v>
@@ -4402,7 +4318,7 @@
         <v>80</v>
       </c>
       <c r="E81" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F81" t="s">
         <v>14</v>
@@ -4413,7 +4329,7 @@
         <v>81</v>
       </c>
       <c r="E82" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F82" t="s">
         <v>14</v>
@@ -4424,7 +4340,7 @@
         <v>82</v>
       </c>
       <c r="E83" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
         <v>14</v>
@@ -4435,7 +4351,7 @@
         <v>83</v>
       </c>
       <c r="E84" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F84" t="s">
         <v>14</v>
@@ -4446,7 +4362,7 @@
         <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F85" t="s">
         <v>14</v>
@@ -4457,7 +4373,7 @@
         <v>85</v>
       </c>
       <c r="E86" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
@@ -4468,7 +4384,7 @@
         <v>86</v>
       </c>
       <c r="E87" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F87" t="s">
         <v>14</v>
@@ -4479,7 +4395,7 @@
         <v>87</v>
       </c>
       <c r="E88" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F88" t="s">
         <v>14</v>
@@ -4490,7 +4406,7 @@
         <v>88</v>
       </c>
       <c r="E89" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F89" t="s">
         <v>14</v>
@@ -4501,7 +4417,7 @@
         <v>89</v>
       </c>
       <c r="E90" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F90" t="s">
         <v>14</v>
@@ -4512,7 +4428,7 @@
         <v>90</v>
       </c>
       <c r="E91" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
@@ -4523,7 +4439,7 @@
         <v>91</v>
       </c>
       <c r="E92" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>
@@ -4534,7 +4450,7 @@
         <v>92</v>
       </c>
       <c r="E93" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F93" t="s">
         <v>14</v>
@@ -4545,7 +4461,7 @@
         <v>93</v>
       </c>
       <c r="E94" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F94" t="s">
         <v>14</v>
@@ -4556,7 +4472,7 @@
         <v>94</v>
       </c>
       <c r="E95" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F95" t="s">
         <v>14</v>
@@ -4567,7 +4483,7 @@
         <v>95</v>
       </c>
       <c r="E96" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F96" t="s">
         <v>14</v>
@@ -4578,7 +4494,7 @@
         <v>96</v>
       </c>
       <c r="E97" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F97" t="s">
         <v>14</v>
@@ -4589,7 +4505,7 @@
         <v>97</v>
       </c>
       <c r="E98" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F98" t="s">
         <v>14</v>
@@ -4600,7 +4516,7 @@
         <v>98</v>
       </c>
       <c r="E99" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F99" t="s">
         <v>14</v>
@@ -4611,7 +4527,7 @@
         <v>99</v>
       </c>
       <c r="E100" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F100" t="s">
         <v>14</v>
@@ -4622,7 +4538,7 @@
         <v>100</v>
       </c>
       <c r="E101" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F101" t="s">
         <v>14</v>

</xml_diff>